<commit_message>
adding columns for plotting
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA_EOT.xlsx
+++ b/data_2023/time_bins/SALMA_EOT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t xml:space="preserve">epoch</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">max_ma</t>
   </si>
   <si>
+    <t xml:space="preserve">abbr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
@@ -43,10 +49,19 @@
     <t xml:space="preserve">GAP</t>
   </si>
   <si>
+    <t xml:space="preserve">#000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oligocene</t>
   </si>
   <si>
     <t xml:space="preserve">Deseadan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ffffb2</t>
   </si>
   <si>
     <r>
@@ -75,9 +90,21 @@
     <t xml:space="preserve">La Cantera</t>
   </si>
   <si>
+    <t xml:space="preserve">La C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#fecc5c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tinguirirican</t>
   </si>
   <si>
+    <t xml:space="preserve">Tin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#fd8d3c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eocene-Oligocene</t>
   </si>
   <si>
@@ -87,10 +114,28 @@
     <t xml:space="preserve">Mustersan</t>
   </si>
   <si>
+    <t xml:space="preserve">Mus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#deebf7</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barrancan</t>
   </si>
   <si>
+    <t xml:space="preserve">Bar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#c6dbef</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vacan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vac.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9ecae1</t>
   </si>
   <si>
     <r>
@@ -119,10 +164,28 @@
     <t xml:space="preserve">Sapoan Fauna</t>
   </si>
   <si>
+    <t xml:space="preserve">Sap.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#6baed6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Riochican</t>
   </si>
   <si>
+    <t xml:space="preserve">Rio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#4292c6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Itaboraian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ita.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#2171b5</t>
   </si>
   <si>
     <t xml:space="preserve">Paleocene-Eocene</t>
@@ -135,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,6 +242,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -234,7 +302,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +316,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,15 +404,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -352,13 +428,19 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>21</v>
@@ -366,13 +448,17 @@
       <c r="D2" s="2" t="n">
         <v>24.2</v>
       </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>24.2</v>
@@ -380,16 +466,22 @@
       <c r="D3" s="3" t="n">
         <v>29.4</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>29.4</v>
@@ -397,13 +489,17 @@
       <c r="D4" s="2" t="n">
         <v>30.617</v>
       </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>30.617</v>
@@ -411,16 +507,22 @@
       <c r="D5" s="3" t="n">
         <v>30.77</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>30.77</v>
@@ -428,13 +530,17 @@
       <c r="D6" s="2" t="n">
         <v>31.3</v>
       </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>31.3</v>
@@ -442,16 +548,22 @@
       <c r="D7" s="3" t="n">
         <v>33.6</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>33.6</v>
@@ -459,13 +571,17 @@
       <c r="D8" s="2" t="n">
         <v>38</v>
       </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>38</v>
@@ -473,16 +589,22 @@
       <c r="D9" s="3" t="n">
         <v>38.2</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>39</v>
@@ -490,13 +612,17 @@
       <c r="D10" s="2" t="n">
         <v>38.2</v>
       </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>39</v>
@@ -504,16 +630,22 @@
       <c r="D11" s="3" t="n">
         <v>41.7</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>41.7</v>
@@ -521,13 +653,17 @@
       <c r="D12" s="2" t="n">
         <v>44</v>
       </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>44</v>
@@ -535,16 +671,22 @@
       <c r="D13" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>46</v>
@@ -552,13 +694,17 @@
       <c r="D14" s="2" t="n">
         <v>47</v>
       </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>47</v>
@@ -566,16 +712,22 @@
       <c r="D15" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>49</v>
@@ -583,13 +735,17 @@
       <c r="D16" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>50</v>
@@ -597,16 +753,22 @@
       <c r="D17" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>51</v>
@@ -614,13 +776,17 @@
       <c r="D18" s="2" t="n">
         <v>52</v>
       </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>52</v>
@@ -628,16 +794,22 @@
       <c r="D19" s="3" t="n">
         <v>54</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>54</v>
@@ -645,11 +817,15 @@
       <c r="D20" s="2" t="n">
         <v>59.2</v>
       </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
extend mustersan : 38.2-38 => 38.2-35
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA_EOT.xlsx
+++ b/data_2023/time_bins/SALMA_EOT.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -552,7 +552,7 @@
         <v>33.6</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
@@ -567,7 +567,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>38.2</v>
@@ -588,10 +588,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>39</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>38.2</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">

</xml_diff>

<commit_message>
added abbr for Mustersan
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/SALMA_EOT.xlsx
+++ b/data_2023/time_bins/SALMA_EOT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t xml:space="preserve">epoch</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mustersan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mus.</t>
   </si>
   <si>
     <t xml:space="preserve">#deebf7</t>
@@ -392,7 +395,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,9 +575,11 @@
       <c r="D9" s="3" t="n">
         <v>38.2</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>14</v>
@@ -603,7 +608,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>39</v>
@@ -612,10 +617,10 @@
         <v>41.7</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>14</v>
@@ -644,7 +649,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>44</v>
@@ -653,13 +658,13 @@
         <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +690,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>47</v>
@@ -694,13 +699,13 @@
         <v>49</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,7 +731,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>50</v>
@@ -735,13 +740,13 @@
         <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +772,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>52</v>
@@ -776,18 +781,18 @@
         <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>

</xml_diff>